<commit_message>
some major changes and partially optimised code
</commit_message>
<xml_diff>
--- a/test-output/ExcelReport/ExtentExcel.xlsx
+++ b/test-output/ExcelReport/ExtentExcel.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="101">
   <si>
     <t>Duration</t>
   </si>
@@ -189,61 +189,55 @@
     <t>device</t>
   </si>
   <si>
-    <t>Sept 30, 2024 7:22:57 pm</t>
-  </si>
-  <si>
-    <t>Sept 30, 2024 7:13:51 pm</t>
-  </si>
-  <si>
-    <t>Sept 30, 2024 7:22:51 pm</t>
-  </si>
-  <si>
-    <t>8 m 59.389 s</t>
+    <t>Oct 04, 2024 7:38:55 pm</t>
+  </si>
+  <si>
+    <t>Oct 04, 2024 7:32:14 pm</t>
+  </si>
+  <si>
+    <t>Oct 04, 2024 7:38:49 pm</t>
+  </si>
+  <si>
+    <t>6 m 34.471 s</t>
   </si>
   <si>
     <t>100%</t>
   </si>
   <si>
-    <t>Successful login with valid credentials</t>
-  </si>
-  <si>
-    <t>33.189 s</t>
+    <t>SETUP: Open Application And Login to the System</t>
+  </si>
+  <si>
+    <t>16.512 s</t>
   </si>
   <si>
     <t>Pharmacist Login</t>
   </si>
   <si>
-    <t>Login with invalid password and verify error message</t>
-  </si>
-  <si>
-    <t>28.401 s</t>
-  </si>
-  <si>
-    <t>Login with invalid email and verify error message</t>
-  </si>
-  <si>
-    <t>27.015 s</t>
+    <t>12.959 s</t>
+  </si>
+  <si>
+    <t>11.522 s</t>
   </si>
   <si>
     <t>Search for a patient by ID and validate the information</t>
   </si>
   <si>
-    <t>43.336 s</t>
+    <t>19.926 s</t>
   </si>
   <si>
     <t>Validating Patients Data, using DataTables and examples</t>
   </si>
   <si>
-    <t>24.728 s</t>
-  </si>
-  <si>
-    <t>24.764 s</t>
+    <t>19.189 s</t>
+  </si>
+  <si>
+    <t>17.589 s</t>
   </si>
   <si>
     <t>Search for a patient by ID and set a review date</t>
   </si>
   <si>
-    <t>27.303 s</t>
+    <t>19.681 s</t>
   </si>
   <si>
     <t>Patient Search Functionality</t>
@@ -252,97 +246,55 @@
     <t>Verify that the Advanced Search popup opens successfully.</t>
   </si>
   <si>
-    <t>22.043 s</t>
+    <t>38.691 s</t>
   </si>
   <si>
     <t>Pharmacist Portal Advance Search Feature</t>
   </si>
   <si>
-    <t>Verify if the results are displayed when user enters First Name</t>
-  </si>
-  <si>
-    <t>21.138 s</t>
-  </si>
-  <si>
-    <t>Verify if the results are displayed when user enters Last Name</t>
-  </si>
-  <si>
-    <t>23.213 s</t>
-  </si>
-  <si>
-    <t>Verify if the results are displayed when user enters FirstName and City</t>
-  </si>
-  <si>
-    <t>22.957 s</t>
-  </si>
-  <si>
-    <t>Error Validation - Verify if the results are displayed when user enters City</t>
-  </si>
-  <si>
-    <t>30.231 s</t>
-  </si>
-  <si>
-    <t>Verify if the results are displayed when user enters FirstName and Selects State</t>
-  </si>
-  <si>
-    <t>20.026 s</t>
-  </si>
-  <si>
-    <t>Error Validation - Verify if the results are displayed when user Selects State</t>
-  </si>
-  <si>
-    <t>18.477 s</t>
-  </si>
-  <si>
-    <t>Verify if the results are displayed when user enters Zip Code</t>
-  </si>
-  <si>
-    <t>19.932 s</t>
-  </si>
-  <si>
-    <t>Negative test scenario - Verify if the results are displayed when user enters Zip Code in invalid format</t>
-  </si>
-  <si>
-    <t>16.146 s</t>
-  </si>
-  <si>
-    <t>Verify if the results are displayed when user enters Phone Number</t>
-  </si>
-  <si>
-    <t>18.755 s</t>
-  </si>
-  <si>
-    <t>Negative test scenario - Verify if the results are displayed when user enters Phone Number in invalid format</t>
-  </si>
-  <si>
-    <t>47.354 s</t>
-  </si>
-  <si>
-    <t>Verify if the results are displayed when user enters Birth Date</t>
-  </si>
-  <si>
-    <t>33.142 s</t>
-  </si>
-  <si>
-    <t>Negative test scenario - Verify if the results are displayed when user enters Birth Date in invalid format</t>
-  </si>
-  <si>
-    <t>18.723 s</t>
-  </si>
-  <si>
-    <t>Enter HPID and verify results</t>
-  </si>
-  <si>
-    <t>17.752 s</t>
-  </si>
-  <si>
-    <t>@testNG</t>
-  </si>
-  <si>
-    <t>@aut_durvesh</t>
-  </si>
-  <si>
-    <t>@dev_windows</t>
+    <t>Verify if the results are displayed when user enters specific Field</t>
+  </si>
+  <si>
+    <t>16.533 s</t>
+  </si>
+  <si>
+    <t>15.048 s</t>
+  </si>
+  <si>
+    <t>15.896 s</t>
+  </si>
+  <si>
+    <t>16.527 s</t>
+  </si>
+  <si>
+    <t>16.559 s</t>
+  </si>
+  <si>
+    <t>15.732 s</t>
+  </si>
+  <si>
+    <t>14.752 s</t>
+  </si>
+  <si>
+    <t>16.220 s</t>
+  </si>
+  <si>
+    <t>Error Validation - Verify if the results are displayed when user enters specific fields</t>
+  </si>
+  <si>
+    <t>29.993 s</t>
+  </si>
+  <si>
+    <t>14.822 s</t>
+  </si>
+  <si>
+    <t>34.743 s</t>
+  </si>
+  <si>
+    <t>15.776 s</t>
+  </si>
+  <si>
+    <t>15.011 s</t>
   </si>
   <si>
     <t>@login</t>
@@ -351,6 +303,9 @@
     <t>@loginFeature</t>
   </si>
   <si>
+    <t>@Setup</t>
+  </si>
+  <si>
     <t>@PatientValScenario</t>
   </si>
   <si>
@@ -363,16 +318,28 @@
     <t>@patientSearchDate</t>
   </si>
   <si>
+    <t>@testScenario4</t>
+  </si>
+  <si>
     <t>@advanceSearch</t>
   </si>
   <si>
-    <t>1 m 28.635 s</t>
-  </si>
-  <si>
-    <t>1 m 32.828 s</t>
-  </si>
-  <si>
-    <t>5 m 29.889 s</t>
+    <t>@testScenario1</t>
+  </si>
+  <si>
+    <t>@testScenario2</t>
+  </si>
+  <si>
+    <t>@testScenario3</t>
+  </si>
+  <si>
+    <t>41.029 s</t>
+  </si>
+  <si>
+    <t>56.704 s</t>
+  </si>
+  <si>
+    <t>4 m 36.318 s</t>
   </si>
 </sst>
 </file>
@@ -1944,13 +1911,13 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>Successful login with valid credentials</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Login with invalid password and verify error message</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Login with invalid email and verify error message</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Search for a patient by ID and validate the information</c:v>
@@ -1968,43 +1935,43 @@
                   <c:v>Verify that the Advanced Search popup opens successfully.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Verify if the results are displayed when user enters First Name</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Verify if the results are displayed when user enters Last Name</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Verify if the results are displayed when user enters FirstName and City</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters City</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Verify if the results are displayed when user enters FirstName and Selects State</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Error Validation - Verify if the results are displayed when user Selects State</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Verify if the results are displayed when user enters Zip Code</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Zip Code in invalid format</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Verify if the results are displayed when user enters Phone Number</c:v>
+                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Phone Number in invalid format</c:v>
+                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Verify if the results are displayed when user enters Birth Date</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Birth Date in invalid format</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Enter HPID and verify results</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2015,64 +1982,64 @@
               <c:numCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>7.0</c:v>
@@ -2136,13 +2103,13 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>Successful login with valid credentials</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Login with invalid password and verify error message</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Login with invalid email and verify error message</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Search for a patient by ID and validate the information</c:v>
@@ -2160,43 +2127,43 @@
                   <c:v>Verify that the Advanced Search popup opens successfully.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Verify if the results are displayed when user enters First Name</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Verify if the results are displayed when user enters Last Name</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Verify if the results are displayed when user enters FirstName and City</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters City</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Verify if the results are displayed when user enters FirstName and Selects State</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Error Validation - Verify if the results are displayed when user Selects State</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Verify if the results are displayed when user enters Zip Code</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Zip Code in invalid format</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Verify if the results are displayed when user enters Phone Number</c:v>
+                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Phone Number in invalid format</c:v>
+                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Verify if the results are displayed when user enters Birth Date</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Birth Date in invalid format</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Enter HPID and verify results</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2263,13 +2230,13 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>Successful login with valid credentials</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Login with invalid password and verify error message</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Login with invalid email and verify error message</c:v>
+                  <c:v>SETUP: Open Application And Login to the System</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Search for a patient by ID and validate the information</c:v>
@@ -2287,43 +2254,43 @@
                   <c:v>Verify that the Advanced Search popup opens successfully.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Verify if the results are displayed when user enters First Name</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Verify if the results are displayed when user enters Last Name</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Verify if the results are displayed when user enters FirstName and City</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters City</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Verify if the results are displayed when user enters FirstName and Selects State</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Error Validation - Verify if the results are displayed when user Selects State</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Verify if the results are displayed when user enters Zip Code</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Zip Code in invalid format</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Verify if the results are displayed when user enters Phone Number</c:v>
+                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Phone Number in invalid format</c:v>
+                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Verify if the results are displayed when user enters Birth Date</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Negative test scenario - Verify if the results are displayed when user enters Birth Date in invalid format</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Enter HPID and verify results</c:v>
+                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2726,76 +2693,88 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$31</c:f>
+              <c:f>Tags!$B$22:$B$33</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>@testNG</c:v>
+                  <c:v>@login</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@aut_durvesh</c:v>
+                  <c:v>@loginFeature</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@dev_windows</c:v>
+                  <c:v>@Setup</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>@login</c:v>
+                  <c:v>@PatientValScenario</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>@loginFeature</c:v>
+                  <c:v>@PatientValidationFeature</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>@PatientValScenario</c:v>
+                  <c:v>@patientSearch</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>@PatientValidationFeature</c:v>
+                  <c:v>@patientSearchDate</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>@patientSearch</c:v>
+                  <c:v>@testScenario4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>@patientSearchDate</c:v>
+                  <c:v>@advanceSearch</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>@advanceSearch</c:v>
+                  <c:v>@testScenario1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>@testScenario2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>@testScenario3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$D$22:$D$31</c:f>
+              <c:f>Tags!$D$22:$D$33</c:f>
               <c:numCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.0</c:v>
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2853,45 +2832,51 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$31</c:f>
+              <c:f>Tags!$B$22:$B$33</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>@testNG</c:v>
+                  <c:v>@login</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@aut_durvesh</c:v>
+                  <c:v>@loginFeature</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@dev_windows</c:v>
+                  <c:v>@Setup</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>@login</c:v>
+                  <c:v>@PatientValScenario</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>@loginFeature</c:v>
+                  <c:v>@PatientValidationFeature</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>@PatientValScenario</c:v>
+                  <c:v>@patientSearch</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>@PatientValidationFeature</c:v>
+                  <c:v>@patientSearchDate</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>@patientSearch</c:v>
+                  <c:v>@testScenario4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>@patientSearchDate</c:v>
+                  <c:v>@advanceSearch</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>@advanceSearch</c:v>
+                  <c:v>@testScenario1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>@testScenario2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>@testScenario3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$F$22:$F$31</c:f>
+              <c:f>Tags!$F$22:$F$33</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2948,45 +2933,51 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$31</c:f>
+              <c:f>Tags!$B$22:$B$33</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>@testNG</c:v>
+                  <c:v>@login</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@aut_durvesh</c:v>
+                  <c:v>@loginFeature</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@dev_windows</c:v>
+                  <c:v>@Setup</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>@login</c:v>
+                  <c:v>@PatientValScenario</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>@loginFeature</c:v>
+                  <c:v>@PatientValidationFeature</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>@PatientValScenario</c:v>
+                  <c:v>@patientSearch</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>@PatientValidationFeature</c:v>
+                  <c:v>@patientSearchDate</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>@patientSearch</c:v>
+                  <c:v>@testScenario4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>@patientSearchDate</c:v>
+                  <c:v>@advanceSearch</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>@advanceSearch</c:v>
+                  <c:v>@testScenario1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>@testScenario2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>@testScenario3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$E$22:$E$31</c:f>
+              <c:f>Tags!$E$22:$E$33</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -6313,7 +6304,7 @@
     <col min="7" max="7" customWidth="true" width="20.85546875"/>
   </cols>
   <sheetData/>
-  <sheetProtection sheet="true" password="EE6B" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="B73F" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6403,23 +6394,23 @@
         <v>29</v>
       </c>
       <c r="G22" s="57" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H22" s="58" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="I22" s="59"/>
       <c r="J22" s="60"/>
     </row>
     <row r="23">
       <c r="B23" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="56" t="s">
         <v>58</v>
-      </c>
-      <c r="C23" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="56" t="s">
-        <v>59</v>
       </c>
       <c r="E23" s="54" t="s">
         <v>57</v>
@@ -6428,23 +6419,23 @@
         <v>29</v>
       </c>
       <c r="G23" s="57" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H23" s="58" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="I23" s="59"/>
       <c r="J23" s="60"/>
     </row>
     <row r="24">
       <c r="B24" s="54" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C24" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="56" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E24" s="54" t="s">
         <v>57</v>
@@ -6453,351 +6444,351 @@
         <v>29</v>
       </c>
       <c r="G24" s="57" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H24" s="58" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="I24" s="59"/>
       <c r="J24" s="60"/>
     </row>
     <row r="25">
       <c r="B25" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>64</v>
-      </c>
       <c r="F25" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="57" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="H25" s="58" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="I25" s="59"/>
       <c r="J25" s="60"/>
     </row>
     <row r="26">
       <c r="B26" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="54" t="s">
-        <v>64</v>
-      </c>
       <c r="F26" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G26" s="57" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="H26" s="58" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="I26" s="59"/>
       <c r="J26" s="60"/>
     </row>
     <row r="27">
       <c r="B27" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="54" t="s">
-        <v>64</v>
-      </c>
       <c r="F27" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G27" s="57" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="H27" s="58" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="I27" s="59"/>
       <c r="J27" s="60"/>
     </row>
     <row r="28">
       <c r="B28" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="54" t="s">
-        <v>69</v>
-      </c>
       <c r="F28" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G28" s="57" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="H28" s="58" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="I28" s="59"/>
       <c r="J28" s="60"/>
     </row>
     <row r="29">
       <c r="B29" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="54" t="s">
-        <v>72</v>
-      </c>
       <c r="F29" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G29" s="57" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H29" s="58" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I29" s="59"/>
       <c r="J29" s="60"/>
     </row>
     <row r="30">
       <c r="B30" s="54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="56" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E30" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F30" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G30" s="57" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="H30" s="58" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="I30" s="59"/>
       <c r="J30" s="60"/>
     </row>
     <row r="31">
       <c r="B31" s="54" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="56" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E31" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F31" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G31" s="57" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="H31" s="58" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="I31" s="59"/>
       <c r="J31" s="60"/>
     </row>
     <row r="32">
       <c r="B32" s="54" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C32" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="56" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E32" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F32" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G32" s="57" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="H32" s="58" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="I32" s="59"/>
       <c r="J32" s="60"/>
     </row>
     <row r="33">
       <c r="B33" s="54" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C33" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="56" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F33" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G33" s="57" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="H33" s="58" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="I33" s="59"/>
       <c r="J33" s="60"/>
     </row>
     <row r="34">
       <c r="B34" s="54" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C34" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="56" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E34" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F34" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G34" s="57" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="H34" s="58" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="I34" s="59"/>
       <c r="J34" s="60"/>
     </row>
     <row r="35">
       <c r="B35" s="54" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C35" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="56" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E35" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F35" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G35" s="57" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="H35" s="58" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="I35" s="59"/>
       <c r="J35" s="60"/>
     </row>
     <row r="36">
       <c r="B36" s="54" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C36" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="56" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E36" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F36" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G36" s="57" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="H36" s="58" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="I36" s="59"/>
       <c r="J36" s="60"/>
     </row>
     <row r="37">
       <c r="B37" s="54" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C37" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D37" s="56" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E37" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F37" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G37" s="57" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="H37" s="58" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="I37" s="59"/>
       <c r="J37" s="60"/>
     </row>
     <row r="38">
       <c r="B38" s="54" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C38" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="56" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E38" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F38" s="55" t="s">
         <v>29</v>
@@ -6813,41 +6804,41 @@
     </row>
     <row r="39">
       <c r="B39" s="54" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C39" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="56" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E39" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F39" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G39" s="57" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="H39" s="58" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I39" s="59"/>
       <c r="J39" s="60"/>
     </row>
     <row r="40">
       <c r="B40" s="54" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C40" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D40" s="56" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E40" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F40" s="55" t="s">
         <v>29</v>
@@ -6863,41 +6854,41 @@
     </row>
     <row r="41">
       <c r="B41" s="54" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="C41" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="56" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E41" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F41" s="55" t="s">
         <v>29</v>
       </c>
       <c r="G41" s="57" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="H41" s="58" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I41" s="59"/>
       <c r="J41" s="60"/>
     </row>
     <row r="42">
       <c r="B42" s="54" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C42" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D42" s="56" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E42" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F42" s="55" t="s">
         <v>29</v>
@@ -6925,7 +6916,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B20:I64"/>
+  <dimension ref="B20:I78"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="21.0" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
@@ -6973,7 +6964,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s" s="54">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C22" s="57" t="n">
         <v>1.0</v>
@@ -6989,13 +6980,13 @@
     </row>
     <row r="23">
       <c r="B23" s="54" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C23" s="57" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D23" s="58" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E23" s="59"/>
       <c r="F23" s="60"/>
@@ -7005,7 +6996,7 @@
     </row>
     <row r="24">
       <c r="B24" s="54" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C24" s="57" t="n">
         <v>1.0</v>
@@ -7021,13 +7012,13 @@
     </row>
     <row r="25">
       <c r="B25" s="54" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C25" s="57" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D25" s="58" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E25" s="59"/>
       <c r="F25" s="60"/>
@@ -7037,7 +7028,7 @@
     </row>
     <row r="26">
       <c r="B26" s="54" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C26" s="57" t="n">
         <v>3.0</v>
@@ -7053,13 +7044,13 @@
     </row>
     <row r="27">
       <c r="B27" s="54" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C27" s="57" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D27" s="58" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E27" s="59"/>
       <c r="F27" s="60"/>
@@ -7069,13 +7060,13 @@
     </row>
     <row r="28">
       <c r="B28" s="54" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C28" s="57" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D28" s="58" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E28" s="59"/>
       <c r="F28" s="60"/>
@@ -7085,7 +7076,7 @@
     </row>
     <row r="29">
       <c r="B29" s="54" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C29" s="57" t="n">
         <v>1.0</v>
@@ -7101,13 +7092,13 @@
     </row>
     <row r="30">
       <c r="B30" s="54" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C30" s="57" t="n">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c r="D30" s="58" t="n">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c r="E30" s="59"/>
       <c r="F30" s="60"/>
@@ -7117,13 +7108,13 @@
     </row>
     <row r="31">
       <c r="B31" s="54" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C31" s="57" t="n">
-        <v>14.0</v>
+        <v>8.0</v>
       </c>
       <c r="D31" s="58" t="n">
-        <v>14.0</v>
+        <v>8.0</v>
       </c>
       <c r="E31" s="59"/>
       <c r="F31" s="60"/>
@@ -7131,63 +7122,59 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="35" t="s">
+    <row r="32">
+      <c r="B32" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D32" s="58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E32" s="59"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="61" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D33" s="58" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E33" s="59"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="61" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C37" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="36" t="s">
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I35" s="35" t="s">
+      <c r="I37" s="35" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I36" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I37" s="55" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="54" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C38" s="62" t="s">
         <v>57</v>
@@ -7205,7 +7192,7 @@
     </row>
     <row r="39">
       <c r="B39" s="54" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C39" s="62" t="s">
         <v>57</v>
@@ -7222,12 +7209,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="62" t="s">
-        <v>57</v>
-      </c>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
       <c r="D40" s="53"/>
       <c r="E40" s="53"/>
       <c r="F40" s="53"/>
@@ -7247,21 +7230,25 @@
       <c r="F41" s="53"/>
       <c r="G41" s="53"/>
       <c r="H41" s="62" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I41" s="55" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
+      <c r="B42" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="62" t="s">
+        <v>57</v>
+      </c>
       <c r="D42" s="53"/>
       <c r="E42" s="53"/>
       <c r="F42" s="53"/>
       <c r="G42" s="53"/>
       <c r="H42" s="62" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I42" s="55" t="s">
         <v>29</v>
@@ -7269,17 +7256,17 @@
     </row>
     <row r="43">
       <c r="B43" s="54" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C43" s="62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D43" s="53"/>
       <c r="E43" s="53"/>
       <c r="F43" s="53"/>
       <c r="G43" s="53"/>
       <c r="H43" s="62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I43" s="55" t="s">
         <v>29</v>
@@ -7293,7 +7280,7 @@
       <c r="F44" s="53"/>
       <c r="G44" s="53"/>
       <c r="H44" s="62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I44" s="55" t="s">
         <v>29</v>
@@ -7307,7 +7294,7 @@
       <c r="F45" s="53"/>
       <c r="G45" s="53"/>
       <c r="H45" s="62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I45" s="55" t="s">
         <v>29</v>
@@ -7315,17 +7302,17 @@
     </row>
     <row r="46">
       <c r="B46" s="54" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C46" s="62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D46" s="53"/>
       <c r="E46" s="53"/>
       <c r="F46" s="53"/>
       <c r="G46" s="53"/>
       <c r="H46" s="62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I46" s="55" t="s">
         <v>29</v>
@@ -7339,7 +7326,7 @@
       <c r="F47" s="53"/>
       <c r="G47" s="53"/>
       <c r="H47" s="62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I47" s="55" t="s">
         <v>29</v>
@@ -7353,7 +7340,7 @@
       <c r="F48" s="53"/>
       <c r="G48" s="53"/>
       <c r="H48" s="62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I48" s="55" t="s">
         <v>29</v>
@@ -7361,17 +7348,17 @@
     </row>
     <row r="49">
       <c r="B49" s="54" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D49" s="53"/>
       <c r="E49" s="53"/>
       <c r="F49" s="53"/>
       <c r="G49" s="53"/>
       <c r="H49" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I49" s="55" t="s">
         <v>29</v>
@@ -7379,17 +7366,17 @@
     </row>
     <row r="50">
       <c r="B50" s="54" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C50" s="62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D50" s="53"/>
       <c r="E50" s="53"/>
       <c r="F50" s="53"/>
       <c r="G50" s="53"/>
       <c r="H50" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I50" s="55" t="s">
         <v>29</v>
@@ -7397,31 +7384,35 @@
     </row>
     <row r="51">
       <c r="B51" s="54" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D51" s="53"/>
       <c r="E51" s="53"/>
       <c r="F51" s="53"/>
       <c r="G51" s="53"/>
       <c r="H51" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="I51" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
       <c r="D52" s="53"/>
       <c r="E52" s="53"/>
       <c r="F52" s="53"/>
       <c r="G52" s="53"/>
       <c r="H52" s="62" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I52" s="55" t="s">
         <v>29</v>
@@ -7435,7 +7426,7 @@
       <c r="F53" s="53"/>
       <c r="G53" s="53"/>
       <c r="H53" s="62" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I53" s="55" t="s">
         <v>29</v>
@@ -7449,7 +7440,7 @@
       <c r="F54" s="53"/>
       <c r="G54" s="53"/>
       <c r="H54" s="62" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I54" s="55" t="s">
         <v>29</v>
@@ -7463,7 +7454,7 @@
       <c r="F55" s="53"/>
       <c r="G55" s="53"/>
       <c r="H55" s="62" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="I55" s="55" t="s">
         <v>29</v>
@@ -7477,7 +7468,7 @@
       <c r="F56" s="53"/>
       <c r="G56" s="53"/>
       <c r="H56" s="62" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I56" s="55" t="s">
         <v>29</v>
@@ -7491,7 +7482,7 @@
       <c r="F57" s="53"/>
       <c r="G57" s="53"/>
       <c r="H57" s="62" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I57" s="55" t="s">
         <v>29</v>
@@ -7505,7 +7496,7 @@
       <c r="F58" s="53"/>
       <c r="G58" s="53"/>
       <c r="H58" s="62" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="I58" s="55" t="s">
         <v>29</v>
@@ -7519,7 +7510,7 @@
       <c r="F59" s="53"/>
       <c r="G59" s="53"/>
       <c r="H59" s="62" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="I59" s="55" t="s">
         <v>29</v>
@@ -7533,7 +7524,7 @@
       <c r="F60" s="53"/>
       <c r="G60" s="53"/>
       <c r="H60" s="62" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="I60" s="55" t="s">
         <v>29</v>
@@ -7547,7 +7538,7 @@
       <c r="F61" s="53"/>
       <c r="G61" s="53"/>
       <c r="H61" s="62" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I61" s="55" t="s">
         <v>29</v>
@@ -7561,7 +7552,7 @@
       <c r="F62" s="53"/>
       <c r="G62" s="53"/>
       <c r="H62" s="62" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I62" s="55" t="s">
         <v>29</v>
@@ -7575,7 +7566,7 @@
       <c r="F63" s="53"/>
       <c r="G63" s="53"/>
       <c r="H63" s="62" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="I63" s="55" t="s">
         <v>29</v>
@@ -7589,31 +7580,244 @@
       <c r="F64" s="53"/>
       <c r="G64" s="53"/>
       <c r="H64" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I64" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" s="53"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I65" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" s="53"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="53"/>
+      <c r="G66" s="53"/>
+      <c r="H66" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I66" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" s="53"/>
+      <c r="C67" s="53"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="53"/>
+      <c r="G67" s="53"/>
+      <c r="H67" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I67" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" s="53"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="53"/>
+      <c r="E68" s="53"/>
+      <c r="F68" s="53"/>
+      <c r="G68" s="53"/>
+      <c r="H68" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I68" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I69" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" s="53"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="53"/>
+      <c r="H70" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I70" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" s="53"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I71" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" s="53"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I72" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" s="53"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53"/>
+      <c r="G73" s="53"/>
+      <c r="H73" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I73" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D74" s="53"/>
+      <c r="E74" s="53"/>
+      <c r="F74" s="53"/>
+      <c r="G74" s="53"/>
+      <c r="H74" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="I74" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" s="53"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="I75" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="I64" s="55" t="s">
+      <c r="C76" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="53"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I76" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" s="53"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="53"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="53"/>
+      <c r="H77" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I77" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" s="53"/>
+      <c r="C78" s="53"/>
+      <c r="D78" s="53"/>
+      <c r="E78" s="53"/>
+      <c r="F78" s="53"/>
+      <c r="G78" s="53"/>
+      <c r="H78" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I78" s="55" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="23">
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
     <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:G42"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:G41"/>
+    <mergeCell ref="C42:G42"/>
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="C43:G45"/>
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="C46:G48"/>
     <mergeCell ref="C49:G49"/>
     <mergeCell ref="C50:G50"/>
-    <mergeCell ref="B51:B64"/>
-    <mergeCell ref="C51:G64"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="B52:B65"/>
+    <mergeCell ref="C52:G65"/>
+    <mergeCell ref="B66:B73"/>
+    <mergeCell ref="C66:G73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:G75"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="C76:G78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7710,7 +7914,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="56" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E22" s="57" t="n">
         <v>3.0</v>
@@ -7724,23 +7928,23 @@
         <v>54</v>
       </c>
       <c r="J22" s="57" t="n">
-        <v>15.0</v>
+        <v>12.0</v>
       </c>
       <c r="K22" s="58" t="n">
-        <v>15.0</v>
+        <v>12.0</v>
       </c>
       <c r="L22" s="59"/>
       <c r="M22" s="60"/>
     </row>
     <row r="23">
       <c r="B23" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="56" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E23" s="57" t="n">
         <v>3.0</v>
@@ -7754,23 +7958,23 @@
         <v>54</v>
       </c>
       <c r="J23" s="57" t="n">
-        <v>12.0</v>
+        <v>21.0</v>
       </c>
       <c r="K23" s="58" t="n">
-        <v>12.0</v>
+        <v>21.0</v>
       </c>
       <c r="L23" s="59"/>
       <c r="M23" s="60"/>
     </row>
     <row r="24">
       <c r="B24" s="54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="56" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" s="57" t="n">
         <v>1.0</v>
@@ -7784,23 +7988,23 @@
         <v>54</v>
       </c>
       <c r="J24" s="57" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="K24" s="58" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="L24" s="59"/>
       <c r="M24" s="60"/>
     </row>
     <row r="25">
       <c r="B25" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="56" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E25" s="57" t="n">
         <v>14.0</v>
@@ -7814,10 +8018,10 @@
         <v>54</v>
       </c>
       <c r="J25" s="57" t="n">
-        <v>96.0</v>
+        <v>104.0</v>
       </c>
       <c r="K25" s="58" t="n">
-        <v>96.0</v>
+        <v>104.0</v>
       </c>
       <c r="L25" s="59"/>
       <c r="M25" s="60"/>
@@ -7896,7 +8100,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>129.0</v>
+        <v>145.0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7965,7 +8169,7 @@
       </c>
       <c r="H5" t="n" s="0">
         <f>SUM(H2:H4)</f>
-        <v>129.0</v>
+        <v>145.0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added drag and drop feature file
</commit_message>
<xml_diff>
--- a/test-output/ExcelReport/ExtentExcel.xlsx
+++ b/test-output/ExcelReport/ExtentExcel.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
   <si>
     <t>Duration</t>
   </si>
@@ -189,157 +189,55 @@
     <t>device</t>
   </si>
   <si>
-    <t>Oct 04, 2024 7:38:55 pm</t>
-  </si>
-  <si>
-    <t>Oct 04, 2024 7:32:14 pm</t>
-  </si>
-  <si>
-    <t>Oct 04, 2024 7:38:49 pm</t>
-  </si>
-  <si>
-    <t>6 m 34.471 s</t>
+    <t>Oct 08, 2024 12:03:36 pm</t>
+  </si>
+  <si>
+    <t>Oct 08, 2024 12:01:39 pm</t>
+  </si>
+  <si>
+    <t>Oct 08, 2024 12:03:33 pm</t>
+  </si>
+  <si>
+    <t>1 m 53.720 s</t>
   </si>
   <si>
     <t>100%</t>
   </si>
   <si>
-    <t>SETUP: Open Application And Login to the System</t>
-  </si>
-  <si>
-    <t>16.512 s</t>
-  </si>
-  <si>
-    <t>Pharmacist Login</t>
-  </si>
-  <si>
-    <t>12.959 s</t>
-  </si>
-  <si>
-    <t>11.522 s</t>
-  </si>
-  <si>
-    <t>Search for a patient by ID and validate the information</t>
-  </si>
-  <si>
-    <t>19.926 s</t>
-  </si>
-  <si>
-    <t>Validating Patients Data, using DataTables and examples</t>
-  </si>
-  <si>
-    <t>19.189 s</t>
-  </si>
-  <si>
-    <t>17.589 s</t>
-  </si>
-  <si>
-    <t>Search for a patient by ID and set a review date</t>
-  </si>
-  <si>
-    <t>19.681 s</t>
-  </si>
-  <si>
-    <t>Patient Search Functionality</t>
-  </si>
-  <si>
-    <t>Verify that the Advanced Search popup opens successfully.</t>
-  </si>
-  <si>
-    <t>38.691 s</t>
-  </si>
-  <si>
-    <t>Pharmacist Portal Advance Search Feature</t>
-  </si>
-  <si>
-    <t>Verify if the results are displayed when user enters specific Field</t>
-  </si>
-  <si>
-    <t>16.533 s</t>
-  </si>
-  <si>
-    <t>15.048 s</t>
-  </si>
-  <si>
-    <t>15.896 s</t>
-  </si>
-  <si>
-    <t>16.527 s</t>
-  </si>
-  <si>
-    <t>16.559 s</t>
-  </si>
-  <si>
-    <t>15.732 s</t>
-  </si>
-  <si>
-    <t>14.752 s</t>
-  </si>
-  <si>
-    <t>16.220 s</t>
-  </si>
-  <si>
-    <t>Error Validation - Verify if the results are displayed when user enters specific fields</t>
-  </si>
-  <si>
-    <t>29.993 s</t>
-  </si>
-  <si>
-    <t>14.822 s</t>
-  </si>
-  <si>
-    <t>34.743 s</t>
-  </si>
-  <si>
-    <t>15.776 s</t>
-  </si>
-  <si>
-    <t>15.011 s</t>
-  </si>
-  <si>
-    <t>@login</t>
-  </si>
-  <si>
-    <t>@loginFeature</t>
-  </si>
-  <si>
-    <t>@Setup</t>
-  </si>
-  <si>
-    <t>@PatientValScenario</t>
-  </si>
-  <si>
-    <t>@PatientValidationFeature</t>
-  </si>
-  <si>
-    <t>@patientSearch</t>
-  </si>
-  <si>
-    <t>@patientSearchDate</t>
-  </si>
-  <si>
-    <t>@testScenario4</t>
-  </si>
-  <si>
-    <t>@advanceSearch</t>
+    <t>Validate table column order after drag and drop</t>
+  </si>
+  <si>
+    <t>44.040 s</t>
+  </si>
+  <si>
+    <t>Validate drag and drop functionality</t>
+  </si>
+  <si>
+    <t>Validate List order after drag and drop</t>
+  </si>
+  <si>
+    <t>36.520 s</t>
+  </si>
+  <si>
+    <t>Validate reset functionality</t>
+  </si>
+  <si>
+    <t>32.408 s</t>
   </si>
   <si>
     <t>@testScenario1</t>
   </si>
   <si>
+    <t>@DragAndDrop</t>
+  </si>
+  <si>
     <t>@testScenario2</t>
   </si>
   <si>
     <t>@testScenario3</t>
   </si>
   <si>
-    <t>41.029 s</t>
-  </si>
-  <si>
-    <t>56.704 s</t>
-  </si>
-  <si>
-    <t>4 m 36.318 s</t>
+    <t>1 m 52.991 s</t>
   </si>
 </sst>
 </file>
@@ -1907,142 +1805,34 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Scenarios!$B$22:$B$42</c:f>
+              <c:f>Scenarios!$B$22:$B$24</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
+                  <c:v>Validate table column order after drag and drop</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
+                  <c:v>Validate List order after drag and drop</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Search for a patient by ID and set a review date</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Verify that the Advanced Search popup opens successfully.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
+                  <c:v>Validate reset functionality</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenarios!$H$22:$H$42</c:f>
+              <c:f>Scenarios!$H$22:$H$24</c:f>
               <c:numCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2099,78 +1889,24 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Scenarios!$B$22:$B$42</c:f>
+              <c:f>Scenarios!$B$22:$B$24</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
+                  <c:v>Validate table column order after drag and drop</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
+                  <c:v>Validate List order after drag and drop</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Search for a patient by ID and set a review date</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Verify that the Advanced Search popup opens successfully.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
+                  <c:v>Validate reset functionality</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenarios!$J$22:$J$42</c:f>
+              <c:f>Scenarios!$J$22:$J$24</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2226,78 +1962,24 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Scenarios!$B$22:$B$42</c:f>
+              <c:f>Scenarios!$B$22:$B$24</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
+                  <c:v>Validate table column order after drag and drop</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
+                  <c:v>Validate List order after drag and drop</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SETUP: Open Application And Login to the System</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Search for a patient by ID and validate the information</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Search for a patient by ID and set a review date</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Verify that the Advanced Search popup opens successfully.</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Error Validation - Verify if the results are displayed when user enters specific fields</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Verify if the results are displayed when user enters specific Field</c:v>
+                  <c:v>Validate reset functionality</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenarios!$I$22:$I$42</c:f>
+              <c:f>Scenarios!$I$22:$I$24</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2693,43 +2375,19 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$33</c:f>
+              <c:f>Tags!$B$22:$B$25</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>@login</c:v>
+                  <c:v>@testScenario1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@loginFeature</c:v>
+                  <c:v>@DragAndDrop</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@Setup</c:v>
+                  <c:v>@testScenario2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>@PatientValScenario</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>@PatientValidationFeature</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>@patientSearch</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>@patientSearchDate</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>@testScenario4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>@advanceSearch</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>@testScenario1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>@testScenario2</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>@testScenario3</c:v>
                 </c:pt>
               </c:strCache>
@@ -2737,9 +2395,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$D$22:$D$33</c:f>
+              <c:f>Tags!$D$22:$D$25</c:f>
               <c:numCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2750,31 +2408,7 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2832,43 +2466,19 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$33</c:f>
+              <c:f>Tags!$B$22:$B$25</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>@login</c:v>
+                  <c:v>@testScenario1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@loginFeature</c:v>
+                  <c:v>@DragAndDrop</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@Setup</c:v>
+                  <c:v>@testScenario2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>@PatientValScenario</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>@PatientValidationFeature</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>@patientSearch</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>@patientSearchDate</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>@testScenario4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>@advanceSearch</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>@testScenario1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>@testScenario2</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>@testScenario3</c:v>
                 </c:pt>
               </c:strCache>
@@ -2876,7 +2486,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$F$22:$F$33</c:f>
+              <c:f>Tags!$F$22:$F$25</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -2933,43 +2543,19 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tags!$B$22:$B$33</c:f>
+              <c:f>Tags!$B$22:$B$25</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>@login</c:v>
+                  <c:v>@testScenario1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>@loginFeature</c:v>
+                  <c:v>@DragAndDrop</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@Setup</c:v>
+                  <c:v>@testScenario2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>@PatientValScenario</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>@PatientValidationFeature</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>@patientSearch</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>@patientSearchDate</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>@testScenario4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>@advanceSearch</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>@testScenario1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>@testScenario2</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>@testScenario3</c:v>
                 </c:pt>
               </c:strCache>
@@ -2977,7 +2563,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tags!$E$22:$E$33</c:f>
+              <c:f>Tags!$E$22:$E$25</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -3182,40 +2768,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Features!$B$22:$B$25</c:f>
+              <c:f>Features!$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pharmacist Login</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Validating Patients Data, using DataTables and examples</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Patient Search Functionality</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Pharmacist Portal Advance Search Feature</c:v>
+                  <c:v>Validate drag and drop functionality</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Features!$F$22:$F$25</c:f>
+              <c:f>Features!$F$22</c:f>
               <c:numCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3272,27 +2840,18 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Features!$B$22:$B$25</c:f>
+              <c:f>Features!$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pharmacist Login</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Validating Patients Data, using DataTables and examples</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Patient Search Functionality</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Pharmacist Portal Advance Search Feature</c:v>
+                  <c:v>Validate drag and drop functionality</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Features!$H$22:$H$25</c:f>
+              <c:f>Features!$H$22</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -3348,27 +2907,18 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Features!$B$22:$B$25</c:f>
+              <c:f>Features!$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pharmacist Login</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Validating Patients Data, using DataTables and examples</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Patient Search Functionality</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Pharmacist Portal Advance Search Feature</c:v>
+                  <c:v>Validate drag and drop functionality</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Features!$G$22:$G$25</c:f>
+              <c:f>Features!$G$22</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -6304,7 +5854,7 @@
     <col min="7" max="7" customWidth="true" width="20.85546875"/>
   </cols>
   <sheetData/>
-  <sheetProtection sheet="true" password="B73F" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="8291" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6313,7 +5863,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B20:J42"/>
+  <dimension ref="B20:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="21.0" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
@@ -6394,23 +5944,23 @@
         <v>29</v>
       </c>
       <c r="G22" s="57" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="H22" s="58" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="I22" s="59"/>
       <c r="J22" s="60"/>
     </row>
     <row r="23">
       <c r="B23" s="54" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" s="54" t="s">
         <v>57</v>
@@ -6419,23 +5969,23 @@
         <v>29</v>
       </c>
       <c r="G23" s="57" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="H23" s="58" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="I23" s="59"/>
       <c r="J23" s="60"/>
     </row>
     <row r="24">
       <c r="B24" s="54" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C24" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="56" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E24" s="54" t="s">
         <v>57</v>
@@ -6444,463 +5994,13 @@
         <v>29</v>
       </c>
       <c r="G24" s="57" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="H24" s="58" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="I24" s="59"/>
       <c r="J24" s="60"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H25" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I25" s="59"/>
-      <c r="J25" s="60"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G26" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H26" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I26" s="59"/>
-      <c r="J26" s="60"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="56" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H27" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I27" s="59"/>
-      <c r="J27" s="60"/>
-    </row>
-    <row r="28">
-      <c r="B28" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G28" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H28" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I28" s="59"/>
-      <c r="J28" s="60"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29" s="57" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="H29" s="58" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="I29" s="59"/>
-      <c r="J29" s="60"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H30" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I30" s="59"/>
-      <c r="J30" s="60"/>
-    </row>
-    <row r="31">
-      <c r="B31" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H31" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I31" s="59"/>
-      <c r="J31" s="60"/>
-    </row>
-    <row r="32">
-      <c r="B32" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H32" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I32" s="59"/>
-      <c r="J32" s="60"/>
-    </row>
-    <row r="33">
-      <c r="B33" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G33" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H33" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I33" s="59"/>
-      <c r="J33" s="60"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H34" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I34" s="59"/>
-      <c r="J34" s="60"/>
-    </row>
-    <row r="35">
-      <c r="B35" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H35" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I35" s="59"/>
-      <c r="J35" s="60"/>
-    </row>
-    <row r="36">
-      <c r="B36" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H36" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I36" s="59"/>
-      <c r="J36" s="60"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="H37" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I37" s="59"/>
-      <c r="J37" s="60"/>
-    </row>
-    <row r="38">
-      <c r="B38" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G38" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H38" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I38" s="59"/>
-      <c r="J38" s="60"/>
-    </row>
-    <row r="39">
-      <c r="B39" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F39" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G39" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H39" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I39" s="59"/>
-      <c r="J39" s="60"/>
-    </row>
-    <row r="40">
-      <c r="B40" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F40" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G40" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H40" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I40" s="59"/>
-      <c r="J40" s="60"/>
-    </row>
-    <row r="41">
-      <c r="B41" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F41" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H41" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I41" s="59"/>
-      <c r="J41" s="60"/>
-    </row>
-    <row r="42">
-      <c r="B42" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" s="57" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H42" s="58" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I42" s="59"/>
-      <c r="J42" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6916,7 +6016,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B20:I78"/>
+  <dimension ref="B20:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="21.0" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
@@ -6964,7 +6064,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s" s="54">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="C22" s="57" t="n">
         <v>1.0</v>
@@ -6980,7 +6080,7 @@
     </row>
     <row r="23">
       <c r="B23" s="54" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="C23" s="57" t="n">
         <v>3.0</v>
@@ -6996,7 +6096,7 @@
     </row>
     <row r="24">
       <c r="B24" s="54" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C24" s="57" t="n">
         <v>1.0</v>
@@ -7012,13 +6112,13 @@
     </row>
     <row r="25">
       <c r="B25" s="54" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C25" s="57" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D25" s="58" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E25" s="59"/>
       <c r="F25" s="60"/>
@@ -7026,798 +6126,134 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="57" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D26" s="58" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E26" s="59"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="57" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D27" s="58" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E27" s="59"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="57" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D28" s="58" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="57" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="58" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61" t="s">
-        <v>54</v>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="35" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="57" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="D30" s="58" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="C30" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="55" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D31" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="E31" s="59"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61" t="s">
-        <v>54</v>
+        <v>63</v>
+      </c>
+      <c r="C31" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="57" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D32" s="58" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61" t="s">
-        <v>54</v>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="I32" s="55" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="57" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D33" s="58" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E33" s="59"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="61" t="s">
-        <v>54</v>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="I33" s="55" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="35" t="s">
-        <v>22</v>
+    <row r="34">
+      <c r="B34" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="I34" s="55" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="38">
-      <c r="B38" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="62" t="s">
+    <row r="35">
+      <c r="B35" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I38" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I39" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I40" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I41" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="I42" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="62" t="s">
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="I43" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="I44" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="I45" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="I46" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="I47" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="I48" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="I49" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="I50" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="I51" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="I52" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" s="53"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
-      <c r="H53" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I53" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="53"/>
-      <c r="H54" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I54" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" s="53"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="53"/>
-      <c r="H55" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I55" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I56" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="53"/>
-      <c r="H57" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I57" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" s="53"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I58" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="53"/>
-      <c r="H59" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I59" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" s="53"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="53"/>
-      <c r="G60" s="53"/>
-      <c r="H60" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I60" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="B61" s="53"/>
-      <c r="C61" s="53"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="53"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="I61" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" s="53"/>
-      <c r="C62" s="53"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="53"/>
-      <c r="G62" s="53"/>
-      <c r="H62" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="I62" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" s="53"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I63" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" s="53"/>
-      <c r="C64" s="53"/>
-      <c r="D64" s="53"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="53"/>
-      <c r="G64" s="53"/>
-      <c r="H64" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I64" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" s="53"/>
-      <c r="C65" s="53"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="53"/>
-      <c r="G65" s="53"/>
-      <c r="H65" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I65" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" s="53"/>
-      <c r="E66" s="53"/>
-      <c r="F66" s="53"/>
-      <c r="G66" s="53"/>
-      <c r="H66" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I66" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" s="53"/>
-      <c r="C67" s="53"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I67" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" s="53"/>
-      <c r="C68" s="53"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="53"/>
-      <c r="G68" s="53"/>
-      <c r="H68" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I68" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="53"/>
-      <c r="G69" s="53"/>
-      <c r="H69" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I69" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="53"/>
-      <c r="G70" s="53"/>
-      <c r="H70" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I70" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="B71" s="53"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="53"/>
-      <c r="E71" s="53"/>
-      <c r="F71" s="53"/>
-      <c r="G71" s="53"/>
-      <c r="H71" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I71" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" s="53"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="53"/>
-      <c r="E72" s="53"/>
-      <c r="F72" s="53"/>
-      <c r="G72" s="53"/>
-      <c r="H72" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I72" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" s="53"/>
-      <c r="C73" s="53"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="53"/>
-      <c r="G73" s="53"/>
-      <c r="H73" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I73" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C74" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D74" s="53"/>
-      <c r="E74" s="53"/>
-      <c r="F74" s="53"/>
-      <c r="G74" s="53"/>
-      <c r="H74" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="I74" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" s="53"/>
-      <c r="C75" s="53"/>
-      <c r="D75" s="53"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="53"/>
-      <c r="G75" s="53"/>
-      <c r="H75" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="I75" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="C76" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D76" s="53"/>
-      <c r="E76" s="53"/>
-      <c r="F76" s="53"/>
-      <c r="G76" s="53"/>
-      <c r="H76" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I76" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" s="53"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="53"/>
-      <c r="E77" s="53"/>
-      <c r="F77" s="53"/>
-      <c r="G77" s="53"/>
-      <c r="H77" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I77" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" s="53"/>
-      <c r="C78" s="53"/>
-      <c r="D78" s="53"/>
-      <c r="E78" s="53"/>
-      <c r="F78" s="53"/>
-      <c r="G78" s="53"/>
-      <c r="H78" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I78" s="55" t="s">
+      <c r="I35" s="55" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="9">
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:G45"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="B52:B65"/>
-    <mergeCell ref="C52:G65"/>
-    <mergeCell ref="B66:B73"/>
-    <mergeCell ref="C66:G73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:G75"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="C76:G78"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7827,7 +6263,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B18:M25"/>
+  <dimension ref="B18:M22"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="21.0" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
@@ -7914,7 +6350,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="56" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E22" s="57" t="n">
         <v>3.0</v>
@@ -7928,103 +6364,13 @@
         <v>54</v>
       </c>
       <c r="J22" s="57" t="n">
-        <v>12.0</v>
+        <v>28.0</v>
       </c>
       <c r="K22" s="58" t="n">
-        <v>12.0</v>
+        <v>28.0</v>
       </c>
       <c r="L22" s="59"/>
       <c r="M22" s="60"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="57" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F23" s="58" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="G23" s="59"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="J23" s="57" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="K23" s="58" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="L23" s="59"/>
-      <c r="M23" s="60"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="57" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F24" s="58" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G24" s="59"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="J24" s="57" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="K24" s="58" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="L24" s="59"/>
-      <c r="M24" s="60"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="57" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="F25" s="58" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="G25" s="59"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="J25" s="57" t="n">
-        <v>104.0</v>
-      </c>
-      <c r="K25" s="58" t="n">
-        <v>104.0</v>
-      </c>
-      <c r="L25" s="59"/>
-      <c r="M25" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8088,19 +6434,19 @@
         <v>3</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>9</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>21.0</v>
+        <v>3.0</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>12</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>145.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8155,21 +6501,21 @@
       </c>
       <c r="D5" t="n" s="0">
         <f>SUM(D2:D4)</f>
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>20</v>
       </c>
       <c r="F5" t="n" s="0">
         <f>SUM(F2:F4)</f>
-        <v>21.0</v>
+        <v>3.0</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>21</v>
       </c>
       <c r="H5" t="n" s="0">
         <f>SUM(H2:H4)</f>
-        <v>145.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>